<commit_message>
Ajout fonction socre sur question
</commit_message>
<xml_diff>
--- a/Ressources/Framework Routing & Reporting 8.5 - Notes.xlsx
+++ b/Ressources/Framework Routing & Reporting 8.5 - Notes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SimonVigoureux\Documents\VisualStudioCode\Maven\QuizSimon-1.2 - Excel\Ressources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CB9B914-0C7D-4484-8CFC-1F955A39E543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB22437-6D2C-480D-B9AD-6521C51BED85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-3450" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-3525" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Routing &amp; Reporting 8" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1085" uniqueCount="572">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1086" uniqueCount="573">
   <si>
     <t>True</t>
   </si>
@@ -1747,6 +1747,9 @@
   </si>
   <si>
     <t>Web Application Server</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -2305,12 +2308,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="A1:I171" totalsRowShown="0">
-  <autoFilter ref="A1:I171" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="A1:J171" totalsRowShown="0">
+  <autoFilter ref="A1:J171" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I171">
     <sortCondition ref="H1:H171"/>
   </sortState>
-  <tableColumns count="9">
+  <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Question"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="nbreRep"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="A"/>
@@ -2320,6 +2323,7 @@
     <tableColumn id="9" xr3:uid="{E8F5A901-874F-4968-BF10-1F55017DC4B4}" name="Justification"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Theme"/>
     <tableColumn id="8" xr3:uid="{678AB2AB-F4B4-4C57-91E7-A9D9BD8E1D63}" name="Formation"/>
+    <tableColumn id="10" xr3:uid="{C4C92D8F-8229-49BC-A6FD-FA42D6E41218}" name="id"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2622,10 +2626,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I171"/>
+  <dimension ref="A1:J171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A132" workbookViewId="0">
-      <selection activeCell="A162" sqref="A162"/>
+    <sheetView tabSelected="1" topLeftCell="B133" workbookViewId="0">
+      <selection activeCell="K169" sqref="K169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2639,7 +2643,7 @@
     <col min="9" max="9" width="31.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -2667,8 +2671,11 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J1" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>139</v>
       </c>
@@ -2693,8 +2700,11 @@
       <c r="I2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>143</v>
       </c>
@@ -2719,8 +2729,11 @@
       <c r="I3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>132</v>
       </c>
@@ -2742,8 +2755,11 @@
       <c r="I4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>129</v>
       </c>
@@ -2765,8 +2781,11 @@
       <c r="I5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>133</v>
       </c>
@@ -2788,8 +2807,11 @@
       <c r="I6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>148</v>
       </c>
@@ -2814,8 +2836,11 @@
       <c r="I7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>136</v>
       </c>
@@ -2834,8 +2859,11 @@
       <c r="I8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>135</v>
       </c>
@@ -2854,8 +2882,11 @@
       <c r="I9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>149</v>
       </c>
@@ -2880,8 +2911,11 @@
       <c r="I10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>159</v>
       </c>
@@ -2906,8 +2940,11 @@
       <c r="I11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>154</v>
       </c>
@@ -2932,8 +2969,11 @@
       <c r="I12" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>158</v>
       </c>
@@ -2952,8 +2992,11 @@
       <c r="I13" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>177</v>
       </c>
@@ -2978,8 +3021,11 @@
       <c r="I14" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>526</v>
       </c>
@@ -3004,8 +3050,11 @@
       <c r="I15" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>120</v>
       </c>
@@ -3030,8 +3079,11 @@
       <c r="I16" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>181</v>
       </c>
@@ -3056,8 +3108,11 @@
       <c r="I17" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>164</v>
       </c>
@@ -3082,8 +3137,11 @@
       <c r="I18" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>168</v>
       </c>
@@ -3108,8 +3166,11 @@
       <c r="I19" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>173</v>
       </c>
@@ -3131,8 +3192,11 @@
       <c r="I20" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -3151,8 +3215,11 @@
       <c r="I21" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>167</v>
       </c>
@@ -3171,8 +3238,11 @@
       <c r="I22" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>194</v>
       </c>
@@ -3191,8 +3261,11 @@
       <c r="I23" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>189</v>
       </c>
@@ -3217,8 +3290,11 @@
       <c r="I24" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>10</v>
       </c>
@@ -3237,8 +3313,11 @@
       <c r="I25" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>166</v>
       </c>
@@ -3257,8 +3336,11 @@
       <c r="I26" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>525</v>
       </c>
@@ -3283,8 +3365,11 @@
       <c r="I27" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>551</v>
       </c>
@@ -3309,8 +3394,11 @@
       <c r="I28" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>203</v>
       </c>
@@ -3329,8 +3417,11 @@
       <c r="I29" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>200</v>
       </c>
@@ -3349,8 +3440,11 @@
       <c r="I30" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>202</v>
       </c>
@@ -3369,8 +3463,11 @@
       <c r="I31" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>197</v>
       </c>
@@ -3395,8 +3492,11 @@
       <c r="I32" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J32">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>204</v>
       </c>
@@ -3415,8 +3515,11 @@
       <c r="I33" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J33">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>198</v>
       </c>
@@ -3435,8 +3538,11 @@
       <c r="I34" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J34">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>199</v>
       </c>
@@ -3455,8 +3561,11 @@
       <c r="I35" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>201</v>
       </c>
@@ -3475,8 +3584,11 @@
       <c r="I36" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J36">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>569</v>
       </c>
@@ -3495,8 +3607,11 @@
       <c r="I37" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J37">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>210</v>
       </c>
@@ -3521,8 +3636,11 @@
       <c r="I38" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J38">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>207</v>
       </c>
@@ -3547,8 +3665,11 @@
       <c r="I39" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J39">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>213</v>
       </c>
@@ -3567,8 +3688,11 @@
       <c r="I40" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J40">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>228</v>
       </c>
@@ -3593,8 +3717,11 @@
       <c r="I41" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J41">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>216</v>
       </c>
@@ -3619,8 +3746,11 @@
       <c r="I42" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J42">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>527</v>
       </c>
@@ -3639,8 +3769,11 @@
       <c r="I43" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J43">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>528</v>
       </c>
@@ -3659,8 +3792,11 @@
       <c r="I44" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J44">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>214</v>
       </c>
@@ -3685,8 +3821,11 @@
       <c r="I45" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J45">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>221</v>
       </c>
@@ -3711,8 +3850,11 @@
       <c r="I46" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J46">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>235</v>
       </c>
@@ -3731,8 +3873,11 @@
       <c r="I47" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J47">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>238</v>
       </c>
@@ -3751,8 +3896,11 @@
       <c r="I48" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J48">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>240</v>
       </c>
@@ -3777,8 +3925,11 @@
       <c r="I49" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J49">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>239</v>
       </c>
@@ -3803,8 +3954,11 @@
       <c r="I50" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J50">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>562</v>
       </c>
@@ -3829,8 +3983,11 @@
       <c r="I51" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J51">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>562</v>
       </c>
@@ -3855,8 +4012,11 @@
       <c r="I52" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J52">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>275</v>
       </c>
@@ -3881,8 +4041,11 @@
       <c r="I53" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J53">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>285</v>
       </c>
@@ -3907,8 +4070,11 @@
       <c r="I54" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J54">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>538</v>
       </c>
@@ -3933,8 +4099,11 @@
       <c r="I55" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J55">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>253</v>
       </c>
@@ -3953,8 +4122,11 @@
       <c r="I56" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J56">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>245</v>
       </c>
@@ -3973,8 +4145,11 @@
       <c r="I57" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J57">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>281</v>
       </c>
@@ -3999,8 +4174,11 @@
       <c r="I58" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J58">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>246</v>
       </c>
@@ -4025,8 +4203,11 @@
       <c r="I59" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J59">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>250</v>
       </c>
@@ -4051,8 +4232,11 @@
       <c r="I60" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J60">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>261</v>
       </c>
@@ -4077,8 +4261,11 @@
       <c r="I61" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J61">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>260</v>
       </c>
@@ -4103,8 +4290,11 @@
       <c r="I62" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J62">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>273</v>
       </c>
@@ -4129,8 +4319,11 @@
       <c r="I63" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J63">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>259</v>
       </c>
@@ -4155,8 +4348,11 @@
       <c r="I64" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J64">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>258</v>
       </c>
@@ -4181,8 +4377,11 @@
       <c r="I65" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J65">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>289</v>
       </c>
@@ -4207,8 +4406,11 @@
       <c r="I66" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J66">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>116</v>
       </c>
@@ -4230,8 +4432,11 @@
       <c r="I67" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J67">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>252</v>
       </c>
@@ -4250,8 +4455,11 @@
       <c r="I68" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J68">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>299</v>
       </c>
@@ -4276,8 +4484,11 @@
       <c r="I69" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J69">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>124</v>
       </c>
@@ -4302,8 +4513,11 @@
       <c r="I70" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J70">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>294</v>
       </c>
@@ -4328,8 +4542,11 @@
       <c r="I71" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J71">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>304</v>
       </c>
@@ -4354,8 +4571,11 @@
       <c r="I72" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J72">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>539</v>
       </c>
@@ -4380,8 +4600,11 @@
       <c r="I73" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J73">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>540</v>
       </c>
@@ -4406,8 +4629,11 @@
       <c r="I74" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J74">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>311</v>
       </c>
@@ -4432,8 +4658,11 @@
       <c r="I75" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J75">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>319</v>
       </c>
@@ -4455,8 +4684,11 @@
       <c r="I76" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J76">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>310</v>
       </c>
@@ -4475,8 +4707,11 @@
       <c r="I77" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J77">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>314</v>
       </c>
@@ -4501,8 +4736,11 @@
       <c r="I78" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J78">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>309</v>
       </c>
@@ -4523,8 +4761,11 @@
       <c r="I79" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J79">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>324</v>
       </c>
@@ -4549,8 +4790,11 @@
       <c r="I80" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J80">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>338</v>
       </c>
@@ -4575,8 +4819,11 @@
       <c r="I81" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J81">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>334</v>
       </c>
@@ -4601,8 +4848,11 @@
       <c r="I82" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J82">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>339</v>
       </c>
@@ -4627,8 +4877,11 @@
       <c r="I83" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J83">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>344</v>
       </c>
@@ -4653,8 +4906,11 @@
       <c r="I84" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J84">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>329</v>
       </c>
@@ -4679,8 +4935,11 @@
       <c r="I85" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J85">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>375</v>
       </c>
@@ -4705,8 +4964,11 @@
       <c r="I86" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J86">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>361</v>
       </c>
@@ -4731,8 +4993,11 @@
       <c r="I87" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J87">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>366</v>
       </c>
@@ -4757,8 +5022,11 @@
       <c r="I88" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J88">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>393</v>
       </c>
@@ -4783,8 +5051,11 @@
       <c r="I89" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J89">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>385</v>
       </c>
@@ -4809,8 +5080,11 @@
       <c r="I90" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J90">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>386</v>
       </c>
@@ -4835,8 +5109,11 @@
       <c r="I91" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J91">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>384</v>
       </c>
@@ -4861,8 +5138,11 @@
       <c r="I92" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J92">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>356</v>
       </c>
@@ -4887,8 +5167,11 @@
       <c r="I93" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J93">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>346</v>
       </c>
@@ -4913,8 +5196,11 @@
       <c r="I94" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J94">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>387</v>
       </c>
@@ -4939,8 +5225,11 @@
       <c r="I95" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J95">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>388</v>
       </c>
@@ -4965,8 +5254,11 @@
       <c r="I96" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J96">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>351</v>
       </c>
@@ -4985,8 +5277,11 @@
       <c r="I97" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J97">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>370</v>
       </c>
@@ -5011,8 +5306,11 @@
       <c r="I98" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J98">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>352</v>
       </c>
@@ -5037,8 +5335,11 @@
       <c r="I99" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J99">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>570</v>
       </c>
@@ -5063,8 +5364,11 @@
       <c r="I100" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J100">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>399</v>
       </c>
@@ -5083,8 +5387,11 @@
       <c r="I101" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J101">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>402</v>
       </c>
@@ -5103,8 +5410,11 @@
       <c r="I102" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J102">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>550</v>
       </c>
@@ -5129,8 +5439,11 @@
       <c r="I103" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J103">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>415</v>
       </c>
@@ -5152,8 +5465,11 @@
       <c r="I104" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J104">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>417</v>
       </c>
@@ -5175,8 +5491,11 @@
       <c r="I105" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J105">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>409</v>
       </c>
@@ -5201,8 +5520,11 @@
       <c r="I106" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J106">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>405</v>
       </c>
@@ -5227,8 +5549,11 @@
       <c r="I107" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J107">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>77</v>
       </c>
@@ -5253,8 +5578,11 @@
       <c r="I108" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J108">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>82</v>
       </c>
@@ -5279,8 +5607,11 @@
       <c r="I109" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J109">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>83</v>
       </c>
@@ -5305,8 +5636,11 @@
       <c r="I110" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J110">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>473</v>
       </c>
@@ -5331,8 +5665,11 @@
       <c r="I111" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J111">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>67</v>
       </c>
@@ -5357,8 +5694,11 @@
       <c r="I112" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J112">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>531</v>
       </c>
@@ -5377,8 +5717,11 @@
       <c r="I113" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J113">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>476</v>
       </c>
@@ -5397,8 +5740,11 @@
       <c r="I114" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J114">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>487</v>
       </c>
@@ -5423,8 +5769,11 @@
       <c r="I115" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J115">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>431</v>
       </c>
@@ -5449,8 +5798,11 @@
       <c r="I116" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J116">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>436</v>
       </c>
@@ -5475,8 +5827,11 @@
       <c r="I117" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J117">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>464</v>
       </c>
@@ -5501,8 +5856,11 @@
       <c r="I118" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J118">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>469</v>
       </c>
@@ -5527,8 +5885,11 @@
       <c r="I119" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J119">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>530</v>
       </c>
@@ -5550,8 +5911,11 @@
       <c r="I120" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J120">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>423</v>
       </c>
@@ -5576,8 +5940,11 @@
       <c r="I121" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J121">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>115</v>
       </c>
@@ -5602,8 +5969,11 @@
       <c r="I122" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J122">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>84</v>
       </c>
@@ -5628,8 +5998,11 @@
       <c r="I123" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J123">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>85</v>
       </c>
@@ -5654,8 +6027,11 @@
       <c r="I124" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J124">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>472</v>
       </c>
@@ -5680,8 +6056,11 @@
       <c r="I125" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J125">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>453</v>
       </c>
@@ -5706,8 +6085,11 @@
       <c r="I126" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J126">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>456</v>
       </c>
@@ -5732,8 +6114,11 @@
       <c r="I127" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J127">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>72</v>
       </c>
@@ -5752,8 +6137,11 @@
       <c r="I128" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J128">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>97</v>
       </c>
@@ -5772,8 +6160,11 @@
       <c r="I129" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J129">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>100</v>
       </c>
@@ -5792,8 +6183,11 @@
       <c r="I130" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J130">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>107</v>
       </c>
@@ -5812,8 +6206,11 @@
       <c r="I131" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J131">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>533</v>
       </c>
@@ -5832,8 +6229,11 @@
       <c r="I132" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J132">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>475</v>
       </c>
@@ -5852,8 +6252,11 @@
       <c r="I133" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J133">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>426</v>
       </c>
@@ -5878,8 +6281,11 @@
       <c r="I134" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J134">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>471</v>
       </c>
@@ -5904,8 +6310,11 @@
       <c r="I135" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J135">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>524</v>
       </c>
@@ -5930,8 +6339,11 @@
       <c r="I136" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J136">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>108</v>
       </c>
@@ -5953,8 +6365,11 @@
       <c r="I137" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J137">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>112</v>
       </c>
@@ -5973,8 +6388,11 @@
       <c r="I138" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J138">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>92</v>
       </c>
@@ -5999,8 +6417,11 @@
       <c r="I139" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J139">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>52</v>
       </c>
@@ -6025,8 +6446,11 @@
       <c r="I140" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J140">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>529</v>
       </c>
@@ -6048,8 +6472,11 @@
       <c r="I141" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J141">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>90</v>
       </c>
@@ -6074,8 +6501,11 @@
       <c r="I142" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J142">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>532</v>
       </c>
@@ -6097,8 +6527,11 @@
       <c r="I143" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J143">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>470</v>
       </c>
@@ -6123,8 +6556,11 @@
       <c r="I144" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J144">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>484</v>
       </c>
@@ -6146,8 +6582,11 @@
       <c r="I145" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J145">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>57</v>
       </c>
@@ -6172,8 +6611,11 @@
       <c r="I146" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J146">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>71</v>
       </c>
@@ -6192,8 +6634,11 @@
       <c r="I147" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J147">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>98</v>
       </c>
@@ -6212,8 +6657,11 @@
       <c r="I148" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J148">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>474</v>
       </c>
@@ -6232,8 +6680,11 @@
       <c r="I149" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J149">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>556</v>
       </c>
@@ -6258,8 +6709,11 @@
       <c r="I150" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J150">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>556</v>
       </c>
@@ -6284,8 +6738,11 @@
       <c r="I151" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J151">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>507</v>
       </c>
@@ -6310,8 +6767,11 @@
       <c r="I152" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J152">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>491</v>
       </c>
@@ -6330,8 +6790,11 @@
       <c r="I153" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J153">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="154" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>496</v>
       </c>
@@ -6352,8 +6815,11 @@
       <c r="I154" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J154">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>493</v>
       </c>
@@ -6374,8 +6840,11 @@
       <c r="I155" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J155">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>504</v>
       </c>
@@ -6400,8 +6869,11 @@
       <c r="I156" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J156">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="157" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>499</v>
       </c>
@@ -6426,8 +6898,11 @@
       <c r="I157" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J157">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="158" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>492</v>
       </c>
@@ -6446,8 +6921,11 @@
       <c r="I158" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J158">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="159" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>510</v>
       </c>
@@ -6466,8 +6944,11 @@
       <c r="I159" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J159">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="160" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>19</v>
       </c>
@@ -6489,8 +6970,11 @@
       <c r="I160" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J160">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="161" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>47</v>
       </c>
@@ -6515,8 +6999,11 @@
       <c r="I161" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J161">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="162" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>20</v>
       </c>
@@ -6541,8 +7028,11 @@
       <c r="I162" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J162">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="163" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>37</v>
       </c>
@@ -6567,8 +7057,11 @@
       <c r="I163" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J163">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="164" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>42</v>
       </c>
@@ -6593,8 +7086,11 @@
       <c r="I164" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J164">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="165" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>511</v>
       </c>
@@ -6619,8 +7115,11 @@
       <c r="I165" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J165">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="166" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>12</v>
       </c>
@@ -6639,8 +7138,11 @@
       <c r="I166" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J166">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="167" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>32</v>
       </c>
@@ -6665,8 +7167,11 @@
       <c r="I167" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J167">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="168" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>15</v>
       </c>
@@ -6685,8 +7190,11 @@
       <c r="I168" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J168">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="169" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>25</v>
       </c>
@@ -6711,8 +7219,11 @@
       <c r="I169" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J169">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="170" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>30</v>
       </c>
@@ -6731,8 +7242,11 @@
       <c r="I170" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J170">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="171" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>31</v>
       </c>
@@ -6750,6 +7264,9 @@
       </c>
       <c r="I171" t="s">
         <v>9</v>
+      </c>
+      <c r="J171">
+        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>